<commit_message>
Ajustes menores. Mejoras en el EA
</commit_message>
<xml_diff>
--- a/Guion - Presentaciones.xlsx
+++ b/Guion - Presentaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vvalotto/OneDrive/Mi trabajo/Docencia/UNER/Ingeniería de Software en Sistemas Embebidos/Contenido/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vvalotto/OneDrive/Mi trabajo/Docencia/UNER/Ingeniería de Software en Sistemas Embebidos/Contenido/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_789DC3F6AE7E7DA5FDE4362C4A025AC379246F10" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{688EF469-6084-2547-B68B-D751ED45C3A9}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_789DC3F6AE7E7DA5FDE4362C4A025AC379246F10" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{841DC4B1-D0E9-3E47-A9BC-1EA634B1251E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Diapositiva</t>
   </si>
@@ -146,6 +146,42 @@
   </si>
   <si>
     <t>Desarrollar los PCU</t>
+  </si>
+  <si>
+    <t>Modulo 3</t>
+  </si>
+  <si>
+    <t>Principios de la IS y Diseño</t>
+  </si>
+  <si>
+    <t>1 a 20</t>
+  </si>
+  <si>
+    <t>21 a 33</t>
+  </si>
+  <si>
+    <t>Arquitectura - Criterios</t>
+  </si>
+  <si>
+    <t>34 a 54</t>
+  </si>
+  <si>
+    <t>Atributos de Calidad - Escenarios - Arq</t>
+  </si>
+  <si>
+    <t>55 a 78</t>
+  </si>
+  <si>
+    <t>Diseño Detallado</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>Implementacion 1 Entrega - Codigo</t>
+  </si>
+  <si>
+    <t>Mostrar Aquitectura C4 y Modelo de Arquitectura</t>
   </si>
 </sst>
 </file>
@@ -895,16 +931,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1070,7 +1107,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" ref="E12:E18" si="1">+E11+D12</f>
+        <f t="shared" ref="E12:E27" si="1">+E11+D12</f>
         <v>1.3541666666666665</v>
       </c>
     </row>
@@ -1118,49 +1155,173 @@
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="3">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="1"/>
-        <v>1.458333333333333</v>
-      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="3">
-        <v>2.0833333333333332E-2</v>
-      </c>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D17" s="3"/>
       <c r="E17" s="3">
-        <f t="shared" si="1"/>
-        <v>1.4791666666666663</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="1"/>
-        <v>1.4999999999999996</v>
+        <v>0.60416666666666674</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>0.62500000000000011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.64583333333333348</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>0.65625000000000011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="1"/>
+        <v>0.68750000000000011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="1"/>
+        <v>0.71875000000000011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="1"/>
+        <v>0.72916666666666674</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="1"/>
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="1"/>
+        <v>0.79166666666666674</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="3">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>